<commit_message>
Cambiata gestione della colonna Anno in superdettagli
</commit_message>
<xml_diff>
--- a/AAA Files for demo/Input files/Budget.xlsx
+++ b/AAA Files for demo/Input files/Budget.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fperrino\Desktop\KPI UT_LAVORO_LEFO\Ottobre 2025\File_utilizzabili\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592694F4-0D5E-47F4-835F-F8B4A1A211EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD9E509-D868-4A1F-88BE-143B39149200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5610" yWindow="1410" windowWidth="28380" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DoesNotMatter" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$J$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DoesNotMatter!$B$2:$J$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>